<commit_message>
Added Units, Fixed UI notifications not displaying properly
</commit_message>
<xml_diff>
--- a/csv/Lessee Information.xlsx
+++ b/csv/Lessee Information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Documents\cpe106lproj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\drpdayan\LocalRepo\SoftDes\Project\CPE106L-4_E01_4Q2324_Project\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDEFDD5-D469-4426-B297-D8ED41D91A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4029408-412E-4545-9527-3F7160D054A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2745" windowWidth="29040" windowHeight="16440" xr2:uid="{1648F1E8-9317-4811-9F96-4F968195E74C}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{1648F1E8-9317-4811-9F96-4F968195E74C}"/>
   </bookViews>
   <sheets>
     <sheet name="Lessee_Information" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
   <si>
     <t>Unit</t>
   </si>
@@ -50,9 +50,6 @@
     <t>1D</t>
   </si>
   <si>
-    <t>Vacant</t>
-  </si>
-  <si>
     <t>Cherry Lynn Santos</t>
   </si>
   <si>
@@ -207,6 +204,93 @@
   </si>
   <si>
     <t xml:space="preserve">Null </t>
+  </si>
+  <si>
+    <t>4I</t>
+  </si>
+  <si>
+    <t>4J</t>
+  </si>
+  <si>
+    <t>4K</t>
+  </si>
+  <si>
+    <t>4L</t>
+  </si>
+  <si>
+    <t>2I</t>
+  </si>
+  <si>
+    <t>2J</t>
+  </si>
+  <si>
+    <t>2K</t>
+  </si>
+  <si>
+    <t>2L</t>
+  </si>
+  <si>
+    <t>3I</t>
+  </si>
+  <si>
+    <t>3J</t>
+  </si>
+  <si>
+    <t>3K</t>
+  </si>
+  <si>
+    <t>3L</t>
+  </si>
+  <si>
+    <t>Cris Dione Sigua</t>
+  </si>
+  <si>
+    <t>Angie Villarico</t>
+  </si>
+  <si>
+    <t>Ronwaldo Bariuan</t>
+  </si>
+  <si>
+    <t>Cecille Espiritu</t>
+  </si>
+  <si>
+    <t>Arvin de Guzman</t>
+  </si>
+  <si>
+    <t>Carissa Tapang</t>
+  </si>
+  <si>
+    <t>Misie Quimba</t>
+  </si>
+  <si>
+    <t>Jennifer Valenzuela</t>
+  </si>
+  <si>
+    <t>Clarissa Gallardo</t>
+  </si>
+  <si>
+    <t>Aaron Alfonso</t>
+  </si>
+  <si>
+    <t>Rowena Barcelona</t>
+  </si>
+  <si>
+    <t>Jonald Cajilig</t>
+  </si>
+  <si>
+    <t>Rhodora Capulong</t>
+  </si>
+  <si>
+    <t>Philip Sevilla</t>
+  </si>
+  <si>
+    <t>Karren Ralutin</t>
+  </si>
+  <si>
+    <t>Zaida Rosales</t>
+  </si>
+  <si>
+    <t>Marvin Inocencio</t>
   </si>
 </sst>
 </file>
@@ -256,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,6 +348,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABFF785-3CFC-489E-B3D5-1512BAF44CD5}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,29 +708,38 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1">
         <v>212584345001</v>
@@ -649,10 +750,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1">
         <v>210326936000</v>
@@ -663,349 +764,517 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
+        <v>60</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
+        <v>61</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
+        <v>62</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
+        <v>63</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>56</v>
+        <v>12</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" t="s">
-        <v>56</v>
+        <v>14</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
+        <v>41</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
+        <v>43</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>28</v>
+        <v>64</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>28</v>
+        <v>65</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>28</v>
+        <v>66</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>56</v>
       </c>
-      <c r="C29" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" t="s">
-        <v>56</v>
+      <c r="B38" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>